<commit_message>
Implemented generateSupplyList() in the absences processor.
</commit_message>
<xml_diff>
--- a/Worksheet_Processing/Workbook-Term2017-2018W.xlsx
+++ b/Worksheet_Processing/Workbook-Term2017-2018W.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="30">
   <si>
     <t>Period 1</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>KD</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>sue</t>
+  </si>
+  <si>
+    <t>idk</t>
   </si>
 </sst>
 </file>
@@ -706,7 +715,7 @@
   <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -797,10 +806,14 @@
       <c r="Y2" s="26"/>
       <c r="Z2" s="26"/>
       <c r="AA2" s="26"/>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-    </row>
-    <row r="3" spans="1:29" ht="54" x14ac:dyDescent="0.2">
+      <c r="AB2" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC2" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="53" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -882,8 +895,12 @@
       <c r="AA3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
+      <c r="AB3" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC3" s="24">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -955,8 +972,12 @@
       <c r="AA4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="24"/>
+      <c r="AB4" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC4" s="24">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">

</xml_diff>

<commit_message>
WorkbookWriter creates a new updated on call tally based on an individual on call. Since the class is not copying the colors from the original spreadsheet, you can pass a path for the output file, so the original wont get lost.
</commit_message>
<xml_diff>
--- a/Worksheet_Processing/Workbook-Term2017-2018W.xlsx
+++ b/Worksheet_Processing/Workbook-Term2017-2018W.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="993" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Schedule" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Week 1" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Week 2" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Week 3" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="etc.." sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Schedule" r:id="rId2" sheetId="1" state="visible"/>
+    <sheet name="Week 1" r:id="rId3" sheetId="2" state="visible"/>
+    <sheet name="Week 2" r:id="rId4" sheetId="3" state="visible"/>
+    <sheet name="Week 3" r:id="rId5" sheetId="4" state="visible"/>
+    <sheet name="etc.." r:id="rId6" sheetId="5" state="visible"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterate="false" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -204,77 +204,77 @@
     </fill>
   </fills>
   <borders count="11">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right style="thin"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right style="thin"/>
       <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right style="thin"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right style="thin"/>
       <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right/>
       <top/>
@@ -283,147 +283,147 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="27">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="7" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="90" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="8" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="9" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -433,18 +433,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E6" activeCellId="0" pane="topLeft" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8279069767442"/>
+    <col min="1" max="1025" hidden="false" style="0" width="10.8279069767442" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +468,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -494,7 +494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -520,7 +520,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="4">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -546,7 +546,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -566,7 +566,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -586,7 +586,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="7">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -594,7 +594,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="8">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -602,7 +602,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="9">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -610,7 +610,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="10">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -618,7 +618,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="11">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -626,7 +626,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="12">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -634,7 +634,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="13">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -642,7 +642,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="14">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -650,7 +650,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="15">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -658,7 +658,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="16">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -666,7 +666,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="17">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -678,9 +678,9 @@
   <mergeCells count="1">
     <mergeCell ref="H1:I1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -693,23 +693,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC29"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.78604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="27" min="3" style="0" width="3.2"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="10.8279069767442"/>
+    <col min="1" max="1" hidden="false" style="0" width="5.78604651162791" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="10.3395348837209" collapsed="true"/>
+    <col min="3" max="27" hidden="false" style="0" width="3.2" collapsed="true"/>
+    <col min="28" max="28" hidden="false" style="0" width="6.27441860465116" collapsed="true"/>
+    <col min="29" max="29" hidden="false" style="0" width="5.16744186046512" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="10.8279069767442" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="1">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="8" t="s">
@@ -746,7 +746,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="2">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="2" t="s">
@@ -787,7 +787,7 @@
       <c r="AB2" s="10"/>
       <c r="AC2" s="10"/>
     </row>
-    <row r="3" customFormat="false" ht="53" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53" outlineLevel="0" r="3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -872,7 +872,7 @@
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -953,7 +953,7 @@
       <c r="AB4" s="10"/>
       <c r="AC4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -1036,7 +1036,7 @@
       <c r="AB5" s="10"/>
       <c r="AC5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -1119,7 +1119,7 @@
       <c r="AB6" s="10"/>
       <c r="AC6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
@@ -1204,7 +1204,7 @@
       <c r="AB7" s="10"/>
       <c r="AC7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
@@ -1285,7 +1285,7 @@
       <c r="AB8" s="10"/>
       <c r="AC8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="9">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="20"/>
@@ -1316,7 +1316,7 @@
       <c r="AB9" s="10"/>
       <c r="AC9" s="10"/>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="10">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="20"/>
@@ -1347,7 +1347,7 @@
       <c r="AB10" s="10"/>
       <c r="AC10" s="10"/>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="11">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="20"/>
@@ -1378,7 +1378,7 @@
       <c r="AB11" s="10"/>
       <c r="AC11" s="10"/>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="12">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="20"/>
@@ -1409,7 +1409,7 @@
       <c r="AB12" s="23"/>
       <c r="AC12" s="23"/>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="13">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="20"/>
@@ -1438,7 +1438,7 @@
       <c r="Z13" s="21"/>
       <c r="AA13" s="22"/>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="14">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -1467,7 +1467,7 @@
       <c r="Z14" s="7"/>
       <c r="AA14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="15">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -1496,7 +1496,7 @@
       <c r="Z15" s="7"/>
       <c r="AA15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="16">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -1525,7 +1525,7 @@
       <c r="Z16" s="7"/>
       <c r="AA16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="17">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -1554,7 +1554,7 @@
       <c r="Z17" s="7"/>
       <c r="AA17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="18">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -1583,7 +1583,7 @@
       <c r="Z18" s="7"/>
       <c r="AA18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="19">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -1612,7 +1612,7 @@
       <c r="Z19" s="7"/>
       <c r="AA19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="20">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -1641,7 +1641,7 @@
       <c r="Z20" s="7"/>
       <c r="AA20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="21">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
@@ -1670,7 +1670,7 @@
       <c r="Z21" s="7"/>
       <c r="AA21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="22">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
@@ -1699,7 +1699,7 @@
       <c r="Z22" s="7"/>
       <c r="AA22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="23">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -1728,7 +1728,7 @@
       <c r="Z23" s="7"/>
       <c r="AA23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="24">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -1757,7 +1757,7 @@
       <c r="Z24" s="7"/>
       <c r="AA24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="25">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -1786,7 +1786,7 @@
       <c r="Z25" s="7"/>
       <c r="AA25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="26">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
@@ -1815,7 +1815,7 @@
       <c r="Z26" s="7"/>
       <c r="AA26" s="6"/>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="27">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -1844,7 +1844,7 @@
       <c r="Z27" s="7"/>
       <c r="AA27" s="6"/>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="28">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
@@ -1873,7 +1873,7 @@
       <c r="Z28" s="7"/>
       <c r="AA28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="29">
       <c r="A29" s="24"/>
       <c r="B29" s="25"/>
       <c r="C29" s="26"/>
@@ -1910,9 +1910,9 @@
     <mergeCell ref="R2:V2"/>
     <mergeCell ref="W2:AA2"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1925,23 +1925,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC41"/>
+  <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="AB2" activeCellId="0" pane="topLeft" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.78604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="27" min="3" style="0" width="3.2"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="10.8279069767442"/>
+    <col min="1" max="1" hidden="false" style="0" width="5.78604651162791" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="10.3395348837209" collapsed="true"/>
+    <col min="3" max="27" hidden="false" style="0" width="3.2" collapsed="true"/>
+    <col min="28" max="28" hidden="false" style="0" width="6.27441860465116" collapsed="true"/>
+    <col min="29" max="29" hidden="false" style="0" width="5.16744186046512" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="10.8279069767442" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="1">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="8" t="s">
@@ -1978,7 +1978,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="2">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="2" t="s">
@@ -2019,7 +2019,7 @@
       <c r="AB2" s="10"/>
       <c r="AC2" s="10"/>
     </row>
-    <row r="3" customFormat="false" ht="53" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53" outlineLevel="0" r="3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2104,7 +2104,7 @@
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -2139,7 +2139,7 @@
       <c r="AB4" s="10"/>
       <c r="AC4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="5">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="13"/>
@@ -2170,7 +2170,7 @@
       <c r="AB5" s="10"/>
       <c r="AC5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="6">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="13"/>
@@ -2201,7 +2201,7 @@
       <c r="AB6" s="10"/>
       <c r="AC6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="7">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="13"/>
@@ -2232,7 +2232,7 @@
       <c r="AB7" s="10"/>
       <c r="AC7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="8">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="17"/>
@@ -2263,7 +2263,7 @@
       <c r="AB8" s="10"/>
       <c r="AC8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="9">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="20"/>
@@ -2294,7 +2294,7 @@
       <c r="AB9" s="10"/>
       <c r="AC9" s="10"/>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="10">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="20"/>
@@ -2325,7 +2325,7 @@
       <c r="AB10" s="10"/>
       <c r="AC10" s="10"/>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="11">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="20"/>
@@ -2356,7 +2356,7 @@
       <c r="AB11" s="10"/>
       <c r="AC11" s="10"/>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="12">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="20"/>
@@ -2387,7 +2387,7 @@
       <c r="AB12" s="23"/>
       <c r="AC12" s="23"/>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="13">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="20"/>
@@ -2416,7 +2416,7 @@
       <c r="Z13" s="21"/>
       <c r="AA13" s="22"/>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="14">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -2445,7 +2445,7 @@
       <c r="Z14" s="7"/>
       <c r="AA14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="15">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -2474,7 +2474,7 @@
       <c r="Z15" s="7"/>
       <c r="AA15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="16">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -2503,7 +2503,7 @@
       <c r="Z16" s="7"/>
       <c r="AA16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="17">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -2532,7 +2532,7 @@
       <c r="Z17" s="7"/>
       <c r="AA17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="18">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -2561,7 +2561,7 @@
       <c r="Z18" s="7"/>
       <c r="AA18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="19">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -2590,7 +2590,7 @@
       <c r="Z19" s="7"/>
       <c r="AA19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="20">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -2619,7 +2619,7 @@
       <c r="Z20" s="7"/>
       <c r="AA20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="21">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
@@ -2648,7 +2648,7 @@
       <c r="Z21" s="7"/>
       <c r="AA21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="22">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
@@ -2677,7 +2677,7 @@
       <c r="Z22" s="7"/>
       <c r="AA22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="23">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -2706,7 +2706,7 @@
       <c r="Z23" s="7"/>
       <c r="AA23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="24">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -2735,7 +2735,7 @@
       <c r="Z24" s="7"/>
       <c r="AA24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="25">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -2764,7 +2764,7 @@
       <c r="Z25" s="7"/>
       <c r="AA25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="26">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
@@ -2793,7 +2793,7 @@
       <c r="Z26" s="7"/>
       <c r="AA26" s="6"/>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="27">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -2822,7 +2822,7 @@
       <c r="Z27" s="7"/>
       <c r="AA27" s="6"/>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="28">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
@@ -2851,7 +2851,7 @@
       <c r="Z28" s="7"/>
       <c r="AA28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="29">
       <c r="A29" s="24"/>
       <c r="B29" s="25"/>
       <c r="C29" s="26"/>
@@ -2880,7 +2880,7 @@
       <c r="Z29" s="25"/>
       <c r="AA29" s="24"/>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="30">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -2888,47 +2888,47 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="31">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="32">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="33">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="34">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="36">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="37">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="38">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="39">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="40">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="41">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
     </row>
@@ -2940,9 +2940,9 @@
     <mergeCell ref="R2:V2"/>
     <mergeCell ref="W2:AA2"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2955,23 +2955,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC41"/>
+  <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC5" activeCellId="0" sqref="AC5"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="AC5" activeCellId="0" pane="topLeft" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.78604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="27" min="3" style="0" width="3.2"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="10.8279069767442"/>
+    <col min="1" max="1" hidden="false" style="0" width="5.78604651162791" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="10.3395348837209" collapsed="true"/>
+    <col min="3" max="27" hidden="false" style="0" width="3.2" collapsed="true"/>
+    <col min="28" max="28" hidden="false" style="0" width="6.27441860465116" collapsed="true"/>
+    <col min="29" max="29" hidden="false" style="0" width="5.16744186046512" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="10.8279069767442" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="1">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="8" t="s">
@@ -3008,7 +3008,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="2">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="2" t="s">
@@ -3049,7 +3049,7 @@
       <c r="AB2" s="10"/>
       <c r="AC2" s="10"/>
     </row>
-    <row r="3" customFormat="false" ht="53" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53" outlineLevel="0" r="3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -3134,7 +3134,7 @@
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -3169,7 +3169,7 @@
       <c r="AB4" s="10"/>
       <c r="AC4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="5">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="13"/>
@@ -3200,7 +3200,7 @@
       <c r="AB5" s="10"/>
       <c r="AC5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="6">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="13"/>
@@ -3231,7 +3231,7 @@
       <c r="AB6" s="10"/>
       <c r="AC6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="7">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="13"/>
@@ -3262,7 +3262,7 @@
       <c r="AB7" s="10"/>
       <c r="AC7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="8">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="17"/>
@@ -3293,7 +3293,7 @@
       <c r="AB8" s="10"/>
       <c r="AC8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="9">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="20"/>
@@ -3324,7 +3324,7 @@
       <c r="AB9" s="10"/>
       <c r="AC9" s="10"/>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="10">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="20"/>
@@ -3355,7 +3355,7 @@
       <c r="AB10" s="10"/>
       <c r="AC10" s="10"/>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="11">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="20"/>
@@ -3386,7 +3386,7 @@
       <c r="AB11" s="10"/>
       <c r="AC11" s="10"/>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="12">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="20"/>
@@ -3417,7 +3417,7 @@
       <c r="AB12" s="23"/>
       <c r="AC12" s="23"/>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="13">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="20"/>
@@ -3446,7 +3446,7 @@
       <c r="Z13" s="21"/>
       <c r="AA13" s="22"/>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="14">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -3475,7 +3475,7 @@
       <c r="Z14" s="7"/>
       <c r="AA14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="15">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -3504,7 +3504,7 @@
       <c r="Z15" s="7"/>
       <c r="AA15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="16">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -3533,7 +3533,7 @@
       <c r="Z16" s="7"/>
       <c r="AA16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="17">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -3562,7 +3562,7 @@
       <c r="Z17" s="7"/>
       <c r="AA17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="18">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -3591,7 +3591,7 @@
       <c r="Z18" s="7"/>
       <c r="AA18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="19">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -3620,7 +3620,7 @@
       <c r="Z19" s="7"/>
       <c r="AA19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="20">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -3649,7 +3649,7 @@
       <c r="Z20" s="7"/>
       <c r="AA20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="21">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
@@ -3678,7 +3678,7 @@
       <c r="Z21" s="7"/>
       <c r="AA21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="22">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
@@ -3707,7 +3707,7 @@
       <c r="Z22" s="7"/>
       <c r="AA22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="23">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -3736,7 +3736,7 @@
       <c r="Z23" s="7"/>
       <c r="AA23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="24">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -3765,7 +3765,7 @@
       <c r="Z24" s="7"/>
       <c r="AA24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="25">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -3794,7 +3794,7 @@
       <c r="Z25" s="7"/>
       <c r="AA25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="26">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
@@ -3823,7 +3823,7 @@
       <c r="Z26" s="7"/>
       <c r="AA26" s="6"/>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="27">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -3852,7 +3852,7 @@
       <c r="Z27" s="7"/>
       <c r="AA27" s="6"/>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="28">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
@@ -3881,7 +3881,7 @@
       <c r="Z28" s="7"/>
       <c r="AA28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="29">
       <c r="A29" s="24"/>
       <c r="B29" s="25"/>
       <c r="C29" s="26"/>
@@ -3910,7 +3910,7 @@
       <c r="Z29" s="25"/>
       <c r="AA29" s="24"/>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="30">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -3918,47 +3918,47 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="31">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="32">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="33">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="34">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="36">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="37">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="38">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="39">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="40">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="41">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
     </row>
@@ -3970,9 +3970,9 @@
     <mergeCell ref="R2:V2"/>
     <mergeCell ref="W2:AA2"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3987,18 +3987,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8279069767442"/>
+    <col min="1" max="1025" hidden="false" style="0" width="10.8279069767442" collapsed="true"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
On Call list now includes supplies and is output to text file
</commit_message>
<xml_diff>
--- a/Worksheet_Processing/Workbook-Term2017-2018W.xlsx
+++ b/Worksheet_Processing/Workbook-Term2017-2018W.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -461,9 +461,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5674418604651"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -717,17 +714,16 @@
   <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD13" activeCellId="0" sqref="AD13"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.02790697674419"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="27" min="3" style="0" width="3.44651162790698"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="27" min="3" style="0" width="3.69302325581395"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.76744186046512"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,9 +1078,7 @@
       <c r="F6" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>42</v>
-      </c>
+      <c r="G6" s="16"/>
       <c r="H6" s="13" t="s">
         <v>42</v>
       </c>
@@ -1159,9 +1153,7 @@
       <c r="B7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>42</v>
-      </c>
+      <c r="C7" s="13"/>
       <c r="D7" s="15" t="s">
         <v>42</v>
       </c>
@@ -1256,9 +1248,7 @@
       <c r="F8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="G8" s="19"/>
       <c r="H8" s="13" t="s">
         <v>42</v>
       </c>
@@ -1978,12 +1968,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.02790697674419"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="27" min="3" style="0" width="3.44651162790698"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="27" min="3" style="0" width="3.69302325581395"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.76744186046512"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3006,12 +2995,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.02790697674419"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="27" min="3" style="0" width="3.44651162790698"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="27" min="3" style="0" width="3.69302325581395"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.76744186046512"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4033,9 +4021,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5674418604651"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Finished Auto-Assigning supply teachers
</commit_message>
<xml_diff>
--- a/Worksheet_Processing/Workbook-Term2017-2018W.xlsx
+++ b/Worksheet_Processing/Workbook-Term2017-2018W.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>IDK</t>
+  </si>
+  <si>
+    <t>Another</t>
   </si>
 </sst>
 </file>
@@ -907,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -998,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="53" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="54" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -1080,8 +1083,12 @@
       <c r="AA3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
+      <c r="AB3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC3" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -1117,9 +1124,7 @@
       <c r="K4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="15" t="s">
-        <v>42</v>
-      </c>
+      <c r="L4" s="15"/>
       <c r="M4" s="12" t="s">
         <v>42</v>
       </c>
@@ -1187,7 +1192,9 @@
       <c r="F5" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="15">
+        <v>2</v>
+      </c>
       <c r="H5" s="12" t="s">
         <v>42</v>
       </c>
@@ -1426,12 +1433,8 @@
       <c r="B8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="16">
-        <v>1</v>
-      </c>
-      <c r="D8" s="17">
-        <v>1</v>
-      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="17" t="s">
         <v>42</v>
       </c>

</xml_diff>